<commit_message>
Add training.py to train space models
</commit_message>
<xml_diff>
--- a/twin4build/test/data/configuration_template_1space_BS2023.xlsx
+++ b/twin4build/test/data/configuration_template_1space_BS2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syddanskuni-my.sharepoint.com/personal/jabj_mmmi_sdu_dk/Documents/PhD_Project_Jakob/Twin4build/python/BuildingEnergyModel/BuildingEnergyModel/twin4build/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{8660571A-4163-4FFB-91CA-F6ABE8F4478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64B6AA59-0F8E-4A2E-B024-1D12A69AE559}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{8660571A-4163-4FFB-91CA-F6ABE8F4478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3732EBB-12C3-4F3E-B203-ECFC16F199BC}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-105" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="3" r:id="rId1"/>
@@ -101,12 +101,6 @@
   </si>
   <si>
     <t>Cooling system name</t>
-  </si>
-  <si>
-    <t>Heating1</t>
-  </si>
-  <si>
-    <t>Ventilation1</t>
   </si>
   <si>
     <t>thermalMassHeatCapacity</t>
@@ -283,9 +277,6 @@
     <t>isContainedIn</t>
   </si>
   <si>
-    <t>Ventilation1;Heating1</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -452,6 +443,15 @@
   </si>
   <si>
     <t>Heating coil temperature sensor;Heat recovery temperature sensor</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>V1;H1</t>
   </si>
 </sst>
 </file>
@@ -678,6 +678,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -979,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B0F6D5-8A47-48C4-A8B6-AFC37A61DB0A}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,10 +1007,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1041,43 +1045,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="L1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="13" t="s">
         <v>97</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1112,80 +1116,80 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" t="s">
         <v>117</v>
       </c>
-      <c r="B3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1232,33 +1236,33 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
         <v>101</v>
       </c>
-      <c r="B2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" t="s">
-        <v>104</v>
-      </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1306,66 +1310,66 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1406,7 +1410,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -1421,67 +1425,67 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1502,12 +1506,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1539,21 +1543,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C2">
         <v>466.54</v>
@@ -1609,102 +1613,102 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="R2">
         <f>4800/3600*1.225</f>
@@ -1713,22 +1717,22 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R3">
         <f t="shared" ref="R3" si="0">4800/3600*1.225</f>
@@ -6771,76 +6775,76 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="P1" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L2">
         <f>3*515+2*572</f>
         <v>2689</v>
       </c>
       <c r="N2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P2">
         <f>125000</f>
@@ -12821,60 +12825,60 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G2">
         <f>5*0.468</f>
@@ -22223,7 +22227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4B0EA7-434A-4CA3-97FE-A57E5232E2E7}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -22238,36 +22242,36 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -28279,54 +28283,54 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I2">
         <f>25000/3600*1.225</f>
@@ -34353,49 +34357,49 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -40376,16 +40380,16 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -40393,16 +40397,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add all changes at earlier commit
</commit_message>
<xml_diff>
--- a/twin4build/test/data/configuration_template_1space_BS2023.xlsx
+++ b/twin4build/test/data/configuration_template_1space_BS2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syddanskuni-my.sharepoint.com/personal/jabj_mmmi_sdu_dk/Documents/PhD_Project_Jakob/Twin4build/python/BuildingEnergyModel/BuildingEnergyModel/twin4build/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{8660571A-4163-4FFB-91CA-F6ABE8F4478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64B6AA59-0F8E-4A2E-B024-1D12A69AE559}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{8660571A-4163-4FFB-91CA-F6ABE8F4478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3732EBB-12C3-4F3E-B203-ECFC16F199BC}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-105" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="3" r:id="rId1"/>
@@ -101,12 +101,6 @@
   </si>
   <si>
     <t>Cooling system name</t>
-  </si>
-  <si>
-    <t>Heating1</t>
-  </si>
-  <si>
-    <t>Ventilation1</t>
   </si>
   <si>
     <t>thermalMassHeatCapacity</t>
@@ -283,9 +277,6 @@
     <t>isContainedIn</t>
   </si>
   <si>
-    <t>Ventilation1;Heating1</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -452,6 +443,15 @@
   </si>
   <si>
     <t>Heating coil temperature sensor;Heat recovery temperature sensor</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>V1;H1</t>
   </si>
 </sst>
 </file>
@@ -678,6 +678,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -979,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B0F6D5-8A47-48C4-A8B6-AFC37A61DB0A}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,10 +1007,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1041,43 +1045,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="L1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="13" t="s">
         <v>97</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1112,80 +1116,80 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" t="s">
         <v>117</v>
       </c>
-      <c r="B3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1232,33 +1236,33 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
         <v>101</v>
       </c>
-      <c r="B2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" t="s">
-        <v>104</v>
-      </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1306,66 +1310,66 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1406,7 +1410,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -1421,67 +1425,67 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1502,12 +1506,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1539,21 +1543,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C2">
         <v>466.54</v>
@@ -1609,102 +1613,102 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="R2">
         <f>4800/3600*1.225</f>
@@ -1713,22 +1717,22 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R3">
         <f t="shared" ref="R3" si="0">4800/3600*1.225</f>
@@ -6771,76 +6775,76 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="P1" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L2">
         <f>3*515+2*572</f>
         <v>2689</v>
       </c>
       <c r="N2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P2">
         <f>125000</f>
@@ -12821,60 +12825,60 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G2">
         <f>5*0.468</f>
@@ -22223,7 +22227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4B0EA7-434A-4CA3-97FE-A57E5232E2E7}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -22238,36 +22242,36 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -28279,54 +28283,54 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I2">
         <f>25000/3600*1.225</f>
@@ -34353,49 +34357,49 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -40376,16 +40380,16 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -40393,16 +40397,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add all changes before re-comitting
</commit_message>
<xml_diff>
--- a/twin4build/test/data/configuration_template_1space_BS2023.xlsx
+++ b/twin4build/test/data/configuration_template_1space_BS2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syddanskuni-my.sharepoint.com/personal/jabj_mmmi_sdu_dk/Documents/PhD_Project_Jakob/Twin4build/python/BuildingEnergyModel/BuildingEnergyModel/twin4build/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{8660571A-4163-4FFB-91CA-F6ABE8F4478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64B6AA59-0F8E-4A2E-B024-1D12A69AE559}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{8660571A-4163-4FFB-91CA-F6ABE8F4478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3732EBB-12C3-4F3E-B203-ECFC16F199BC}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-105" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="3" r:id="rId1"/>
@@ -101,12 +101,6 @@
   </si>
   <si>
     <t>Cooling system name</t>
-  </si>
-  <si>
-    <t>Heating1</t>
-  </si>
-  <si>
-    <t>Ventilation1</t>
   </si>
   <si>
     <t>thermalMassHeatCapacity</t>
@@ -283,9 +277,6 @@
     <t>isContainedIn</t>
   </si>
   <si>
-    <t>Ventilation1;Heating1</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -452,6 +443,15 @@
   </si>
   <si>
     <t>Heating coil temperature sensor;Heat recovery temperature sensor</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>V1;H1</t>
   </si>
 </sst>
 </file>
@@ -678,6 +678,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -979,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B0F6D5-8A47-48C4-A8B6-AFC37A61DB0A}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,10 +1007,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1041,43 +1045,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="L1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="13" t="s">
         <v>97</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1112,80 +1116,80 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" t="s">
         <v>117</v>
       </c>
-      <c r="B3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1232,33 +1236,33 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
         <v>101</v>
       </c>
-      <c r="B2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" t="s">
-        <v>104</v>
-      </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1306,66 +1310,66 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1406,7 +1410,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -1421,67 +1425,67 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1502,12 +1506,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1539,21 +1543,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C2">
         <v>466.54</v>
@@ -1609,102 +1613,102 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="R2">
         <f>4800/3600*1.225</f>
@@ -1713,22 +1717,22 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R3">
         <f t="shared" ref="R3" si="0">4800/3600*1.225</f>
@@ -6771,76 +6775,76 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="P1" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L2">
         <f>3*515+2*572</f>
         <v>2689</v>
       </c>
       <c r="N2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P2">
         <f>125000</f>
@@ -12821,60 +12825,60 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G2">
         <f>5*0.468</f>
@@ -22223,7 +22227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4B0EA7-434A-4CA3-97FE-A57E5232E2E7}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -22238,36 +22242,36 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -28279,54 +28283,54 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I2">
         <f>25000/3600*1.225</f>
@@ -34353,49 +34357,49 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -40376,16 +40380,16 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -40393,16 +40397,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add password protected link to time series data
</commit_message>
<xml_diff>
--- a/twin4build/test/data/configuration_template_1space_BS2023.xlsx
+++ b/twin4build/test/data/configuration_template_1space_BS2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syddanskuni-my.sharepoint.com/personal/jabj_mmmi_sdu_dk/Documents/PhD_Project_Jakob/Twin4build/python/BuildingEnergyModel/BuildingEnergyModel/twin4build/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="8_{8660571A-4163-4FFB-91CA-F6ABE8F4478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71C24616-608C-4317-8AF4-C600E92AC839}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="8_{8660571A-4163-4FFB-91CA-F6ABE8F4478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB9F6173-A611-4FB8-9182-7E1484E7B311}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
   </bookViews>
@@ -6747,7 +6747,7 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6836,8 +6836,8 @@
         <v>101</v>
       </c>
       <c r="L2">
-        <f>(3*515+2*572)/5</f>
-        <v>537.79999999999995</v>
+        <f>(3*515+2*572)</f>
+        <v>2689</v>
       </c>
       <c r="N2" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Move to python 3.10.12 and add OU44 room model
</commit_message>
<xml_diff>
--- a/twin4build/test/data/configuration_template_1space_BS2023.xlsx
+++ b/twin4build/test/data/configuration_template_1space_BS2023.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="86" documentId="8_{8660571A-4163-4FFB-91CA-F6ABE8F4478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB9F6173-A611-4FB8-9182-7E1484E7B311}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
+    <workbookView xWindow="-38520" yWindow="-105" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="3" r:id="rId1"/>

</xml_diff>